<commit_message>
Rename Test Case List Of Symbol
</commit_message>
<xml_diff>
--- a/cypress/downloads/fund_assets.xlsx
+++ b/cypress/downloads/fund_assets.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,145 +427,283 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>شستا</v>
+        <v>وسپهر</v>
       </c>
       <c r="B2" t="str">
-        <v>شرکتهای چند رشته ای صنعتی</v>
+        <v>سرمایه گذاریها</v>
       </c>
       <c r="C2">
-        <v>383040000000</v>
+        <v>56069000000</v>
       </c>
       <c r="D2">
-        <v>1.1183032892</v>
+        <v>1.5561182349</v>
       </c>
       <c r="E2">
-        <v>0.1004933494</v>
+        <v>0.1819371276</v>
       </c>
       <c r="F2">
-        <v>0.02407942</v>
+        <v>0.01769802</v>
       </c>
       <c r="G2">
-        <v>23.76821915</v>
+        <v>2.84611454</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>تاپیکو</v>
+        <v>وبصادر</v>
       </c>
       <c r="B3" t="str">
-        <v>محصولات شیمیایی</v>
+        <v>بانک ها، موسسات اعتباری و سایر نهادهای پولی</v>
       </c>
       <c r="C3">
-        <v>423570000000</v>
+        <v>48833099640</v>
       </c>
       <c r="D3">
-        <v>1.3141933514</v>
+        <v>1.5014039866</v>
       </c>
       <c r="E3">
-        <v>0.1214666973</v>
+        <v>0.1453584896</v>
       </c>
       <c r="F3">
-        <v>0.03023869</v>
+        <v>0.01593854</v>
       </c>
       <c r="G3">
-        <v>26.28316778</v>
+        <v>2.47881351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>حکشتی</v>
+        <v>تیپیکو</v>
       </c>
       <c r="B4" t="str">
-        <v>حمل و نقل، انبارداری و ارتباطات</v>
+        <v>مواد و محصولات دارویی</v>
       </c>
       <c r="C4">
-        <v>462080000000</v>
+        <v>70100000000</v>
       </c>
       <c r="D4">
-        <v>1.2883824768</v>
+        <v>0.7326509394</v>
       </c>
       <c r="E4">
-        <v>0.1348464215</v>
+        <v>0.0784467814</v>
       </c>
       <c r="F4">
-        <v>0.04477942</v>
+        <v>0.01141072</v>
       </c>
       <c r="G4">
-        <v>28.67277231</v>
+        <v>3.55834114</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>وکار</v>
+        <v>وبملت</v>
       </c>
       <c r="B5" t="str">
         <v>بانک ها، موسسات اعتباری و سایر نهادهای پولی</v>
       </c>
       <c r="C5">
-        <v>242428634205</v>
+        <v>58068000000</v>
       </c>
       <c r="D5">
-        <v>0.2952068674</v>
+        <v>0.8856630173</v>
       </c>
       <c r="E5">
-        <v>0.0676030493</v>
+        <v>0.1058060463</v>
       </c>
       <c r="F5">
-        <v>0.0152652</v>
+        <v>0.03747018</v>
       </c>
       <c r="G5">
-        <v>15.04306836</v>
+        <v>2.94758564</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>پاکشو</v>
+        <v>فملی</v>
       </c>
       <c r="B6" t="str">
-        <v>محصولات شیمیایی</v>
+        <v>فلزات اساسی</v>
       </c>
       <c r="C6">
-        <v>51612000000</v>
+        <v>48300000000</v>
       </c>
       <c r="D6">
-        <v>0.3267245052</v>
+        <v>0.823199619</v>
       </c>
       <c r="E6">
-        <v>0.0524019207</v>
+        <v>0.0900707746</v>
       </c>
       <c r="F6">
-        <v>-0.00239513</v>
+        <v>0.0237642</v>
       </c>
       <c r="G6">
-        <v>3.20260371</v>
+        <v>2.45175288</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>وبصادر</v>
+        <v>تاصیکو</v>
       </c>
       <c r="B7" t="str">
+        <v>استخراج کانه های فلزی</v>
+      </c>
+      <c r="C7">
+        <v>31775000000</v>
+      </c>
+      <c r="D7">
+        <v>0.3539362408</v>
+      </c>
+      <c r="E7">
+        <v>0.0582551103</v>
+      </c>
+      <c r="F7">
+        <v>0.02728387</v>
+      </c>
+      <c r="G7">
+        <v>1.61292853</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>سفارس</v>
+      </c>
+      <c r="B8" t="str">
+        <v>سیمان، آهک و گچ</v>
+      </c>
+      <c r="C8">
+        <v>72762500000</v>
+      </c>
+      <c r="D8">
+        <v>0.9621651542</v>
+      </c>
+      <c r="E8">
+        <v>0.1077471765</v>
+      </c>
+      <c r="F8">
+        <v>0.04516604</v>
+      </c>
+      <c r="G8">
+        <v>3.69349211</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>انتخاب</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ماشین آلات و تجهیزات</v>
+      </c>
+      <c r="C9">
+        <v>1016494856340</v>
+      </c>
+      <c r="D9">
+        <v>1.2927220328</v>
+      </c>
+      <c r="E9">
+        <v>0.1345797348</v>
+      </c>
+      <c r="F9">
+        <v>0.01170711</v>
+      </c>
+      <c r="G9">
+        <v>51.59822346</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>شستا</v>
+      </c>
+      <c r="B10" t="str">
+        <v>شرکتهای چند رشته ای صنعتی</v>
+      </c>
+      <c r="C10">
+        <v>52147200000</v>
+      </c>
+      <c r="D10">
+        <v>1.1114061145</v>
+      </c>
+      <c r="E10">
+        <v>0.1040262314</v>
+      </c>
+      <c r="F10">
+        <v>0.02129395</v>
+      </c>
+      <c r="G10">
+        <v>2.64704033</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>وکار</v>
+      </c>
+      <c r="B11" t="str">
         <v>بانک ها، موسسات اعتباری و سایر نهادهای پولی</v>
       </c>
-      <c r="C7">
-        <v>48833099640</v>
-      </c>
-      <c r="D7">
-        <v>1.3316671459</v>
-      </c>
-      <c r="E7">
-        <v>0.1323380095</v>
-      </c>
-      <c r="F7">
-        <v>0.00657324</v>
-      </c>
-      <c r="G7">
-        <v>3.03016869</v>
+      <c r="C11">
+        <v>246819441838</v>
+      </c>
+      <c r="D11">
+        <v>0.4363923146</v>
+      </c>
+      <c r="E11">
+        <v>0.0775113587</v>
+      </c>
+      <c r="F11">
+        <v>0.00328698</v>
+      </c>
+      <c r="G11">
+        <v>12.52878422</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>فباهنر</v>
+      </c>
+      <c r="B12" t="str">
+        <v>فلزات اساسی</v>
+      </c>
+      <c r="C12">
+        <v>15750000000</v>
+      </c>
+      <c r="D12">
+        <v>1.2967432778</v>
+      </c>
+      <c r="E12">
+        <v>0.1546501591</v>
+      </c>
+      <c r="F12">
+        <v>0.03468104</v>
+      </c>
+      <c r="G12">
+        <v>0.79948464</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>فولاد</v>
+      </c>
+      <c r="B13" t="str">
+        <v>فلزات اساسی</v>
+      </c>
+      <c r="C13">
+        <v>252900000000</v>
+      </c>
+      <c r="D13">
+        <v>0.8213573532</v>
+      </c>
+      <c r="E13">
+        <v>0.0843446747</v>
+      </c>
+      <c r="F13">
+        <v>0.01697103</v>
+      </c>
+      <c r="G13">
+        <v>12.837439</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>